<commit_message>
Drawing use case diagram
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoang\OneDrive\Máy tính\TVM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2FFC44-9BDD-4D57-80F3-3E3D2191E7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BED4A21-E6EF-43E8-B0EC-3DB850782B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional Requirements" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>The TVM interface must be easy to use for the majority of users</t>
+  </si>
+  <si>
+    <t>The TVM should have a report issue on the menu</t>
+  </si>
+  <si>
+    <t>The TVM will have a report issue option for user to send the issue to the admin</t>
   </si>
 </sst>
 </file>
@@ -236,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
@@ -252,12 +258,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,21 +641,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="5.5703125" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="49.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="49.88671875" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -669,7 +669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -683,7 +683,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -697,7 +697,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -711,7 +711,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -725,7 +725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>5</v>
       </c>
@@ -739,7 +739,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>6</v>
       </c>
@@ -753,7 +753,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>7</v>
       </c>
@@ -767,7 +767,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>8</v>
       </c>
@@ -781,7 +781,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>9</v>
       </c>
@@ -795,7 +795,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>10</v>
       </c>
@@ -809,7 +809,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>11</v>
       </c>
@@ -823,7 +823,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>12</v>
       </c>
@@ -837,13 +837,21 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <v>13</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
@@ -861,19 +869,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3FAD48F-E9F9-40AA-A425-7C4ADC88BC37}">
   <dimension ref="B4:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" customWidth="1"/>
     <col min="3" max="3" width="42" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
     <col min="5" max="5" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -887,7 +895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <v>1</v>
       </c>
@@ -901,7 +909,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>2</v>
       </c>
@@ -915,7 +923,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>3</v>
       </c>
@@ -929,7 +937,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>4</v>
       </c>
@@ -943,7 +951,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>5</v>
       </c>
@@ -957,7 +965,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>6</v>
       </c>
@@ -971,17 +979,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
-        <v>7</v>
-      </c>
-      <c r="C11" s="6" t="s">
+    <row r="11" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="3">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="6" t="s">
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1001,15 +1009,15 @@
       <selection activeCell="E24" sqref="E23:E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="5.7109375" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="49.7109375" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="49.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -1023,7 +1031,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <v>1</v>
       </c>
@@ -1037,7 +1045,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>2</v>
       </c>
@@ -1051,7 +1059,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>3</v>
       </c>
@@ -1065,7 +1073,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>4</v>
       </c>
@@ -1079,7 +1087,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>5</v>
       </c>
@@ -1093,79 +1101,79 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="4"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="4"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="4"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="4"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="4"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="4"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="4"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="4"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="4"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="4"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="4"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="4"/>

</xml_diff>